<commit_message>
sprints e backlog att
</commit_message>
<xml_diff>
--- a/Documentação/PRODUCT BACKLOG.xlsx
+++ b/Documentação/PRODUCT BACKLOG.xlsx
@@ -62,9 +62,6 @@
     <t>Código do Arduino</t>
   </si>
   <si>
-    <t>Criação do banco no Azure</t>
-  </si>
-  <si>
     <t>Conexão e interação do
 sistema com o banco</t>
   </si>
@@ -140,6 +137,9 @@
   </si>
   <si>
     <t>Gráficos de temperatura e umidade em relação ao tempo, Comparações entre dados de incubadoras diferentes.</t>
+  </si>
+  <si>
+    <t>Desenvolvimento do banco no Azure</t>
   </si>
 </sst>
 </file>
@@ -162,7 +162,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,6 +205,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -292,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -324,6 +330,54 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -339,53 +393,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -675,7 +684,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,15 +698,15 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -708,25 +717,25 @@
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="25" t="s">
+      <c r="G2" s="25" t="s">
         <v>34</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>35</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>20</v>
+      <c r="A3" s="30" t="s">
+        <v>19</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
@@ -734,32 +743,32 @@
       <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="23"/>
+      <c r="D3" s="18"/>
       <c r="E3" s="4"/>
-      <c r="F3" s="26"/>
+      <c r="F3" s="21"/>
       <c r="G3" s="4"/>
       <c r="H3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
+      <c r="A4" s="31"/>
       <c r="B4" s="4">
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="23"/>
+      <c r="D4" s="18"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="26"/>
+      <c r="F4" s="21"/>
       <c r="G4" s="4"/>
       <c r="H4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
+      <c r="A5" s="31"/>
       <c r="B5" s="4">
         <v>3</v>
       </c>
@@ -767,15 +776,15 @@
         <v>8</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="20"/>
+      <c r="E5" s="15"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="18"/>
+      <c r="G5" s="13"/>
       <c r="H5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="8">
         <v>4</v>
       </c>
@@ -784,15 +793,15 @@
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="31"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="26"/>
       <c r="H6" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>21</v>
+      <c r="A7" s="33" t="s">
+        <v>20</v>
       </c>
       <c r="B7" s="6">
         <v>5</v>
@@ -800,156 +809,156 @@
       <c r="C7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="32"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="27"/>
       <c r="H7" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
+      <c r="A8" s="33"/>
       <c r="B8" s="6">
         <v>6</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="21"/>
+        <v>37</v>
+      </c>
+      <c r="D8" s="19"/>
+      <c r="E8" s="16"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
+      <c r="A9" s="33"/>
       <c r="B9" s="4">
         <v>7</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="33"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="28"/>
       <c r="H9" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
+      <c r="A10" s="33"/>
       <c r="B10" s="4">
         <v>8</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="18"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="13"/>
       <c r="H10" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
+      <c r="A11" s="33"/>
       <c r="B11" s="4">
         <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="20"/>
+        <v>17</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="15"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
+      <c r="A12" s="33"/>
       <c r="B12" s="4">
         <v>10</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="18"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="13"/>
       <c r="H12" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
+      <c r="A13" s="33"/>
       <c r="B13" s="4">
         <v>11</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="20"/>
+        <v>22</v>
+      </c>
+      <c r="D13" s="18"/>
+      <c r="E13" s="15"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
+      <c r="A14" s="33"/>
       <c r="B14" s="4">
         <v>12</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="18"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="13"/>
       <c r="H14" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
+      <c r="A15" s="33"/>
       <c r="B15" s="4">
         <v>13</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="18"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="34"/>
       <c r="H15" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
+      <c r="A16" s="33"/>
       <c r="B16" s="4">
         <v>14</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="20"/>
+        <v>25</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="15"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>